<commit_message>
Added division by quarters
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -3,7 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Ответы на форму (1)" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Квартал 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Квартал 2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Квартал 3" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
   <si>
     <t>Отметка времени</t>
   </si>
@@ -25,7 +27,7 @@
     <t>Любовь</t>
   </si>
   <si>
-    <t>Финансы</t>
+    <t>Деньги</t>
   </si>
   <si>
     <t>Работа</t>
@@ -44,6 +46,12 @@
   </si>
   <si>
     <t>Ваши комментарии  или пожелания</t>
+  </si>
+  <si>
+    <t>Отношения</t>
+  </si>
+  <si>
+    <t>Личностный рост</t>
   </si>
   <si>
     <t xml:space="preserve">5 общага самая лучшая </t>
@@ -101,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -110,6 +118,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -124,6 +135,14 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -336,7 +355,7 @@
   <cols>
     <col customWidth="1" min="1" max="10" width="18.88"/>
     <col customWidth="1" min="11" max="11" width="21.5"/>
-    <col customWidth="1" min="12" max="17" width="18.88"/>
+    <col customWidth="1" min="12" max="19" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -352,7 +371,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -372,6 +391,12 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2">
@@ -406,8 +431,10 @@
         <v>10.0</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="3">
       <c r="A3" s="3">
@@ -441,8 +468,10 @@
         <v>10.0</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="4">
       <c r="A4" s="3">
@@ -508,8 +537,10 @@
         <v>10.0</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="3">
@@ -1023,8 +1054,10 @@
         <v>8.0</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>14</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="3">
@@ -1218,8 +1251,10 @@
         <v>5.0</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="3">
@@ -1477,8 +1512,10 @@
         <v>1.0</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
     </row>
     <row r="36">
       <c r="A36" s="3">
@@ -1608,8 +1645,10 @@
         <v>4.0</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
     </row>
     <row r="40">
       <c r="A40" s="3">
@@ -1705,6 +1744,2815 @@
       </c>
       <c r="J42" s="4">
         <v>3.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.88"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>44849.66374270833</v>
+      </c>
+      <c r="B2" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3">
+        <v>44849.66747206019</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>44849.66804138889</v>
+      </c>
+      <c r="B4" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>44849.669849768514</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>44849.70906267361</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>11.0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>44849.71458496527</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>44849.72595304398</v>
+      </c>
+      <c r="B8" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>44849.740629837965</v>
+      </c>
+      <c r="B9" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>44849.74071914352</v>
+      </c>
+      <c r="B10" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3">
+        <v>44849.650609062504</v>
+      </c>
+      <c r="B11" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3">
+        <v>44849.65081378473</v>
+      </c>
+      <c r="B12" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3">
+        <v>44849.651324363425</v>
+      </c>
+      <c r="B13" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3">
+        <v>44849.65222684028</v>
+      </c>
+      <c r="B14" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3">
+        <v>44849.655736458335</v>
+      </c>
+      <c r="B15" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3">
+        <v>44849.65607880787</v>
+      </c>
+      <c r="B16" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3">
+        <v>44849.67073420139</v>
+      </c>
+      <c r="B17" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3">
+        <v>44849.67719325231</v>
+      </c>
+      <c r="B18" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3">
+        <v>44849.68749592593</v>
+      </c>
+      <c r="B19" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3">
+        <v>44849.7019984838</v>
+      </c>
+      <c r="B20" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C20" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3">
+        <v>44849.734627048616</v>
+      </c>
+      <c r="B21" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3">
+        <v>44849.653499305554</v>
+      </c>
+      <c r="B22" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C22" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J22" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3">
+        <v>44849.65448515046</v>
+      </c>
+      <c r="B23" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="I23" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3">
+        <v>44849.65466665509</v>
+      </c>
+      <c r="B24" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="I24" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="J24" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3">
+        <v>44849.655349444445</v>
+      </c>
+      <c r="B25" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3">
+        <v>44849.656906874996</v>
+      </c>
+      <c r="B26" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="I26" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J26" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3">
+        <v>44849.657873738426</v>
+      </c>
+      <c r="B27" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="I27" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J27" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3">
+        <v>44849.658890810184</v>
+      </c>
+      <c r="B28" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H28" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I28" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J28" s="4">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3">
+        <v>44849.659358599536</v>
+      </c>
+      <c r="B29" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C29" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E29" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="I29" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J29" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3">
+        <v>44849.66935972222</v>
+      </c>
+      <c r="B30" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C30" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D30" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E30" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I30" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J30" s="4">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3">
+        <v>44849.671154537034</v>
+      </c>
+      <c r="B31" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C31" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D31" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="E31" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I31" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J31" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3">
+        <v>44849.671359409724</v>
+      </c>
+      <c r="B32" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C32" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E32" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I32" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J32" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3">
+        <v>44849.67190930556</v>
+      </c>
+      <c r="B33" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C33" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E33" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H33" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I33" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J33" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3">
+        <v>44849.68504927083</v>
+      </c>
+      <c r="B34" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C34" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D34" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E34" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H34" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I34" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J34" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3">
+        <v>44849.68775347222</v>
+      </c>
+      <c r="B35" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C35" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="D35" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E35" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F35" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G35" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H35" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I35" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J35" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="3">
+        <v>44849.692041331014</v>
+      </c>
+      <c r="B36" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C36" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D36" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E36" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F36" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G36" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H36" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="I36" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J36" s="4">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3">
+        <v>44849.71684953704</v>
+      </c>
+      <c r="B37" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C37" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E37" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F37" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G37" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H37" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I37" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J37" s="4">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3">
+        <v>44849.76569346065</v>
+      </c>
+      <c r="B38" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C38" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D38" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E38" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F38" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G38" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="H38" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I38" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="J38" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3">
+        <v>44849.78276582176</v>
+      </c>
+      <c r="B39" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C39" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D39" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E39" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="F39" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G39" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H39" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I39" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J39" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="3">
+        <v>44849.78464020834</v>
+      </c>
+      <c r="B40" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C40" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D40" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="E40" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F40" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G40" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H40" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="I40" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J40" s="4">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3">
+        <v>44849.822642858795</v>
+      </c>
+      <c r="B41" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C41" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D41" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E41" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F41" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G41" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H41" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J41" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3">
+        <v>44851.430659317135</v>
+      </c>
+      <c r="B42" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C42" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="D42" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E42" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F42" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G42" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H42" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I42" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J42" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>44849.66374270833</v>
+      </c>
+      <c r="B2" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3">
+        <v>44849.66747206019</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>44849.66804138889</v>
+      </c>
+      <c r="B4" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>44849.669849768514</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>44849.70906267361</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>44849.71458496527</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>44849.72595304398</v>
+      </c>
+      <c r="B8" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>44849.740629837965</v>
+      </c>
+      <c r="B9" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>44849.74071914352</v>
+      </c>
+      <c r="B10" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3">
+        <v>44849.650609062504</v>
+      </c>
+      <c r="B11" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3">
+        <v>44849.65081378473</v>
+      </c>
+      <c r="B12" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3">
+        <v>44849.651324363425</v>
+      </c>
+      <c r="B13" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3">
+        <v>44849.65222684028</v>
+      </c>
+      <c r="B14" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3">
+        <v>44849.655736458335</v>
+      </c>
+      <c r="B15" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3">
+        <v>44849.65607880787</v>
+      </c>
+      <c r="B16" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3">
+        <v>44849.67073420139</v>
+      </c>
+      <c r="B17" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3">
+        <v>44849.67719325231</v>
+      </c>
+      <c r="B18" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3">
+        <v>44849.68749592593</v>
+      </c>
+      <c r="B19" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3">
+        <v>44849.7019984838</v>
+      </c>
+      <c r="B20" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3">
+        <v>44849.734627048616</v>
+      </c>
+      <c r="B21" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3">
+        <v>44849.653499305554</v>
+      </c>
+      <c r="B22" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C22" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J22" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3">
+        <v>44849.65448515046</v>
+      </c>
+      <c r="B23" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I23" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3">
+        <v>44849.65466665509</v>
+      </c>
+      <c r="B24" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I24" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J24" s="4">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3">
+        <v>44849.655349444445</v>
+      </c>
+      <c r="B25" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3">
+        <v>44849.656906874996</v>
+      </c>
+      <c r="B26" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C26" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I26" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J26" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3">
+        <v>44849.657873738426</v>
+      </c>
+      <c r="B27" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C27" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I27" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J27" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3">
+        <v>44849.658890810184</v>
+      </c>
+      <c r="B28" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C28" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H28" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I28" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J28" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3">
+        <v>44849.659358599536</v>
+      </c>
+      <c r="B29" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C29" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E29" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I29" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J29" s="4">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3">
+        <v>44849.66935972222</v>
+      </c>
+      <c r="B30" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C30" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D30" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E30" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I30" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J30" s="4">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3">
+        <v>44849.671154537034</v>
+      </c>
+      <c r="B31" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C31" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D31" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E31" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F31" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I31" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J31" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3">
+        <v>44849.671359409724</v>
+      </c>
+      <c r="B32" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C32" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E32" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="I32" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J32" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3">
+        <v>44849.67190930556</v>
+      </c>
+      <c r="B33" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C33" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D33" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="E33" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="H33" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="I33" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J33" s="4">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3">
+        <v>44849.68504927083</v>
+      </c>
+      <c r="B34" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C34" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="D34" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="E34" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="H34" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="I34" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J34" s="4">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3">
+        <v>44849.68775347222</v>
+      </c>
+      <c r="B35" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C35" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D35" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="E35" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F35" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G35" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="H35" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="I35" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J35" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="3">
+        <v>44849.692041331014</v>
+      </c>
+      <c r="B36" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C36" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D36" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="E36" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F36" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G36" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="H36" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I36" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J36" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3">
+        <v>44849.71684953704</v>
+      </c>
+      <c r="B37" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C37" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="E37" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="F37" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G37" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H37" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="I37" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="J37" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3">
+        <v>44849.76569346065</v>
+      </c>
+      <c r="B38" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C38" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D38" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E38" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F38" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G38" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H38" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="I38" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J38" s="4">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3">
+        <v>44849.78276582176</v>
+      </c>
+      <c r="B39" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C39" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="D39" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E39" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F39" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G39" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="H39" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I39" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="J39" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="3">
+        <v>44849.78464020834</v>
+      </c>
+      <c r="B40" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C40" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D40" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="E40" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F40" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G40" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H40" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="I40" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="J40" s="4">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3">
+        <v>44849.822642858795</v>
+      </c>
+      <c r="B41" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C41" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E41" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F41" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G41" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="H41" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="J41" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3">
+        <v>44851.430659317135</v>
+      </c>
+      <c r="B42" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C42" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="D42" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="E42" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F42" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G42" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="H42" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="I42" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="J42" s="4">
+        <v>7.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>